<commit_message>
Added keepout for usb connector
</commit_message>
<xml_diff>
--- a/LHCbit/LHCbit/BOM/BOM_JLCPCB-LHCbit.xlsx
+++ b/LHCbit/LHCbit/BOM/BOM_JLCPCB-LHCbit.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leand\Documents\Altium\Projetos\LHC\LHCbit\LHCbit\LHCbit\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C4B777D9-12A9-49E7-BD9F-D2D8F85C4F02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B4D15355-1BE4-420E-B6B7-A634F6002062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="4680" windowWidth="38700" windowHeight="15285" xr2:uid="{814D4159-C567-43D9-993B-A2F0A9FDDC2A}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="38700" windowHeight="15285" xr2:uid="{443E0804-E6AE-44AE-8E2D-54130479CC37}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM_JLCPCB-LHCbit" sheetId="1" r:id="rId1"/>
@@ -695,7 +695,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{004E6150-2C85-4689-B15E-1B4B2ABFA25B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C5B777F-0AFD-4E20-9E30-04D30F2E570E}">
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>